<commit_message>
Updating Marissa's office location
</commit_message>
<xml_diff>
--- a/Course Map.xlsx
+++ b/Course Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfdeblasio/Google Drive/Classes/CS2401/cs2401-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4707845B-C66D-7C45-BF5A-0BF2B49F352C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62419135-D03F-304F-879C-2E37AA783684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51740" yWindow="10560" windowWidth="37040" windowHeight="21100" activeTab="1" xr2:uid="{E8B53F2A-050F-7446-94ED-1EBC7A28030C}"/>
+    <workbookView xWindow="9220" yWindow="1100" windowWidth="37040" windowHeight="21100" activeTab="1" xr2:uid="{E8B53F2A-050F-7446-94ED-1EBC7A28030C}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules Topics Objectives" sheetId="1" r:id="rId1"/>
@@ -797,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -930,6 +930,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1406,7 +1409,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="57"/>
-      <c r="B8" s="55">
+      <c r="B8" s="67">
         <v>3</v>
       </c>
       <c r="C8" s="31">
@@ -1613,8 +1616,8 @@
       <c r="G8" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="J8" s="51" t="s">
-        <v>176</v>
+      <c r="J8" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="K8" s="37"/>
     </row>
@@ -1630,14 +1633,14 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="51" t="s">
-        <v>177</v>
+      <c r="J9" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="57"/>
-      <c r="B10" s="49">
+      <c r="B10" s="54">
         <v>4</v>
       </c>
       <c r="C10" s="52">
@@ -1649,8 +1652,8 @@
       <c r="E10" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>12</v>
+      <c r="F10" s="51" t="s">
+        <v>176</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7" t="s">
@@ -1672,8 +1675,8 @@
         <v>48</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="17" t="s">
-        <v>13</v>
+      <c r="F11" s="51" t="s">
+        <v>177</v>
       </c>
       <c r="G11" s="47" t="s">
         <v>175</v>

</xml_diff>

<commit_message>
Starting to update for F22
</commit_message>
<xml_diff>
--- a/Course Map.xlsx
+++ b/Course Map.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfdeblasio/Google Drive/Classes/CS2401/cs2401-documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF15EF3D-A928-A34D-9DCB-FC37B0C1590E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B18F9E0-41DF-4B4D-BDAD-F7F3CACD9C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="3080" windowWidth="26640" windowHeight="21100" activeTab="1" xr2:uid="{E8B53F2A-050F-7446-94ED-1EBC7A28030C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26160" activeTab="1" xr2:uid="{E8B53F2A-050F-7446-94ED-1EBC7A28030C}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules Topics Objectives" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan F21" sheetId="4" r:id="rId2"/>
-    <sheet name="Plan F20" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Plan F22" sheetId="5" r:id="rId2"/>
+    <sheet name="Plan F21" sheetId="4" r:id="rId3"/>
+    <sheet name="Plan F20" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="224">
   <si>
     <t>Week</t>
   </si>
@@ -682,6 +683,33 @@
   </si>
   <si>
     <t xml:space="preserve">Holiday/Video/Marissa? </t>
+  </si>
+  <si>
+    <t>Tuesday Date</t>
+  </si>
+  <si>
+    <t>Tuesday Activities</t>
+  </si>
+  <si>
+    <t>Thursday Acitivies</t>
+  </si>
+  <si>
+    <t>Tuesday Videos</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Lab 0 -- Questionare</t>
+  </si>
+  <si>
+    <t>Setting up Replit</t>
+  </si>
+  <si>
+    <t>Intros</t>
+  </si>
+  <si>
+    <t>n^2 sort (Cont'd)</t>
   </si>
 </sst>
 </file>
@@ -1069,6 +1097,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1102,9 +1133,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1576,10 +1604,692 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3704EE74-89C6-014C-AC77-E74106E27498}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="23.83203125" customWidth="1"/>
+    <col min="7" max="7" width="77.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" customWidth="1"/>
+    <col min="11" max="11" width="45.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="28">
+        <v>44431</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="74"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="32"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="74"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="17"/>
+      <c r="H4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="39" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="74"/>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="29">
+        <v>44438</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="54"/>
+      <c r="H5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="74"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="74"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="19"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="74"/>
+      <c r="B8" s="46">
+        <v>3</v>
+      </c>
+      <c r="C8" s="30">
+        <v>44445</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="54"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="K8" s="34"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="74"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="74"/>
+      <c r="B10" s="45">
+        <v>4</v>
+      </c>
+      <c r="C10" s="44">
+        <v>44452</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="54"/>
+      <c r="H10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="50"/>
+      <c r="F11" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="43"/>
+      <c r="J11" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" s="51"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="6">
+        <v>5</v>
+      </c>
+      <c r="C12" s="30">
+        <v>44459</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="74"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="K13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74"/>
+      <c r="B14" s="42">
+        <v>6</v>
+      </c>
+      <c r="C14" s="29">
+        <v>44466</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="G14" s="37"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="47">
+        <v>7</v>
+      </c>
+      <c r="C15" s="28">
+        <v>44473</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="K15" s="35"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="74"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="48" t="s">
+        <v>191</v>
+      </c>
+      <c r="K16" s="32"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="74"/>
+      <c r="B17" s="42">
+        <v>8</v>
+      </c>
+      <c r="C17" s="29">
+        <v>44480</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="G17" s="37"/>
+      <c r="H17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="11"/>
+      <c r="J17" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="74"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="71" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="32"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="74"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="32"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="74"/>
+      <c r="B20" s="42">
+        <v>9</v>
+      </c>
+      <c r="C20" s="29">
+        <v>44487</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="37"/>
+      <c r="H20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="74"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="74"/>
+      <c r="B22" s="45">
+        <v>10</v>
+      </c>
+      <c r="C22" s="29">
+        <v>44494</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" s="37"/>
+      <c r="H22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="55" t="s">
+        <v>178</v>
+      </c>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="74"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="K23" s="32"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="74"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="32"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="74"/>
+      <c r="B25" s="57">
+        <v>11</v>
+      </c>
+      <c r="C25" s="58">
+        <v>44501</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="59"/>
+      <c r="F25" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="60"/>
+      <c r="H25" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="59"/>
+      <c r="J25" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" s="61"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="74"/>
+      <c r="B26" s="6">
+        <v>12</v>
+      </c>
+      <c r="C26" s="30">
+        <v>44508</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="K26" s="76"/>
+    </row>
+    <row r="27" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="75"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="43" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="43"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="77"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="47">
+        <v>13</v>
+      </c>
+      <c r="C28" s="28">
+        <v>44515</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="36"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="K28" s="62"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="64" t="s">
+        <v>196</v>
+      </c>
+      <c r="K29" s="65"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="57">
+        <v>14</v>
+      </c>
+      <c r="C30" s="58">
+        <v>44522</v>
+      </c>
+      <c r="D30" s="59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="59"/>
+      <c r="F30" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G30" s="60"/>
+      <c r="H30" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="59"/>
+      <c r="J30" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="K30" s="66" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="68">
+        <v>15</v>
+      </c>
+      <c r="C31" s="30">
+        <v>44529</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A27"/>
+    <mergeCell ref="K26:K27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FCF832-66DA-5042-83DC-63C0CD32B871}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -1632,7 +2342,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="73" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="4">
@@ -1663,7 +2373,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="6"/>
       <c r="C3" s="17"/>
       <c r="D3" s="7"/>
@@ -1682,7 +2392,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17"/>
       <c r="D4" s="7"/>
@@ -1701,7 +2411,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="10">
         <v>2</v>
       </c>
@@ -1734,7 +2444,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="6"/>
       <c r="C6" s="17"/>
       <c r="D6" s="7" t="s">
@@ -1757,7 +2467,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="12"/>
       <c r="C7" s="19"/>
       <c r="D7" s="13"/>
@@ -1774,7 +2484,7 @@
       <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="46">
         <v>3</v>
       </c>
@@ -1801,7 +2511,7 @@
       <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="71"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="6"/>
       <c r="C9" s="17"/>
       <c r="D9" s="7" t="s">
@@ -1818,7 +2528,7 @@
       <c r="K9" s="49"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="45">
         <v>4</v>
       </c>
@@ -1847,7 +2557,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="43"/>
       <c r="C11" s="20"/>
       <c r="D11" s="43" t="s">
@@ -1870,7 +2580,7 @@
       <c r="K11" s="51"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="74" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="6">
@@ -1901,7 +2611,7 @@
       <c r="K12" s="32"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="6"/>
       <c r="C13" s="17"/>
       <c r="D13" s="7"/>
@@ -1917,7 +2627,7 @@
       <c r="K13" s="32"/>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="42">
         <v>6</v>
       </c>
@@ -1944,7 +2654,7 @@
       <c r="K14" s="31"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="73" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="47">
@@ -1957,7 +2667,7 @@
         <v>26</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="70" t="s">
         <v>211</v>
       </c>
       <c r="G15" s="36"/>
@@ -1973,12 +2683,12 @@
       <c r="K15" s="35"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="71"/>
+      <c r="A16" s="74"/>
       <c r="B16" s="6"/>
       <c r="C16" s="30"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-      <c r="F16" s="82"/>
+      <c r="F16" s="71"/>
       <c r="G16" s="8"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -1988,7 +2698,7 @@
       <c r="K16" s="32"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="42">
         <v>8</v>
       </c>
@@ -2001,7 +2711,7 @@
       <c r="E17" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="F17" s="83" t="s">
+      <c r="F17" s="72" t="s">
         <v>192</v>
       </c>
       <c r="G17" s="37"/>
@@ -2017,14 +2727,14 @@
       <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="7"/>
       <c r="C18" s="17"/>
       <c r="D18" s="8" t="s">
         <v>123</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="82" t="s">
+      <c r="F18" s="71" t="s">
         <v>193</v>
       </c>
       <c r="G18" s="8"/>
@@ -2034,14 +2744,14 @@
       <c r="K18" s="32"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="71"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="6"/>
       <c r="C19" s="17"/>
       <c r="D19" s="8" t="s">
         <v>179</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="82"/>
+      <c r="F19" s="71"/>
       <c r="G19" s="8"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
@@ -2049,7 +2759,7 @@
       <c r="K19" s="32"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="71"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="42">
         <v>9</v>
       </c>
@@ -2076,7 +2786,7 @@
       <c r="K20" s="31"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="71"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="7"/>
       <c r="C21" s="17"/>
       <c r="D21" s="7"/>
@@ -2089,7 +2799,7 @@
       <c r="K21" s="32"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="71"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="45">
         <v>10</v>
       </c>
@@ -2118,7 +2828,7 @@
       <c r="K22" s="31"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="71"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="6"/>
       <c r="C23" s="17"/>
       <c r="D23" s="7" t="s">
@@ -2137,7 +2847,7 @@
       <c r="K23" s="32"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="71"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="6"/>
       <c r="C24" s="17"/>
       <c r="D24" s="7"/>
@@ -2152,7 +2862,7 @@
       <c r="K24" s="32"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="71"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="57">
         <v>11</v>
       </c>
@@ -2181,7 +2891,7 @@
       <c r="K25" s="61"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="6">
         <v>12</v>
       </c>
@@ -2203,10 +2913,10 @@
       <c r="J26" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="K26" s="73"/>
+      <c r="K26" s="76"/>
     </row>
     <row r="27" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="52"/>
       <c r="C27" s="20"/>
       <c r="D27" s="43" t="s">
@@ -2218,7 +2928,7 @@
       <c r="H27" s="43"/>
       <c r="I27" s="43"/>
       <c r="J27" s="20"/>
-      <c r="K27" s="74"/>
+      <c r="K27" s="77"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
@@ -2327,7 +3037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A478A4-F22F-7A4D-9C9A-0515F98BB5C4}">
   <dimension ref="A1:J29"/>
   <sheetViews>
@@ -2375,7 +3085,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="73" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="4">
@@ -2398,12 +3108,12 @@
       <c r="I2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="80" t="s">
+      <c r="J2" s="83" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="6"/>
       <c r="C3" s="17"/>
       <c r="D3" s="7"/>
@@ -2414,10 +3124,10 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="73"/>
+      <c r="J3" s="76"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="6"/>
       <c r="C4" s="17"/>
       <c r="D4" s="7"/>
@@ -2428,10 +3138,10 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="76"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="10">
         <v>2</v>
       </c>
@@ -2456,12 +3166,12 @@
       <c r="I5" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="78" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="6"/>
       <c r="C6" s="17"/>
       <c r="D6" s="7" t="s">
@@ -2476,10 +3186,10 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="73"/>
+      <c r="J6" s="76"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="12"/>
       <c r="C7" s="19"/>
       <c r="D7" s="13"/>
@@ -2490,10 +3200,10 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="76"/>
+      <c r="J7" s="79"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="6">
         <v>3</v>
       </c>
@@ -2518,12 +3228,12 @@
       <c r="I8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="77" t="s">
+      <c r="J8" s="80" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="71"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="6"/>
       <c r="C9" s="17"/>
       <c r="D9" s="7" t="s">
@@ -2538,10 +3248,10 @@
       <c r="I9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="78"/>
+      <c r="J9" s="81"/>
     </row>
     <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="15">
         <v>4</v>
       </c>
@@ -2562,10 +3272,10 @@
       <c r="I10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="79"/>
+      <c r="J10" s="82"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="73" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="4">
@@ -2590,12 +3300,12 @@
       <c r="I11" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="83" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="71"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="6"/>
       <c r="C12" s="17"/>
       <c r="D12" s="7" t="s">
@@ -2610,10 +3320,10 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="76"/>
+      <c r="J12" s="79"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="10">
         <v>6</v>
       </c>
@@ -2638,12 +3348,12 @@
       <c r="I13" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="J13" s="75" t="s">
+      <c r="J13" s="78" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="6"/>
       <c r="C14" s="17"/>
       <c r="D14" s="7" t="s">
@@ -2656,10 +3366,10 @@
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="17"/>
-      <c r="J14" s="73"/>
+      <c r="J14" s="76"/>
     </row>
     <row r="15" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="6"/>
       <c r="C15" s="17"/>
       <c r="D15" s="7" t="s">
@@ -2670,10 +3380,10 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="74"/>
+      <c r="J15" s="77"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="73" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="4">
@@ -2698,12 +3408,12 @@
       <c r="I16" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="J16" s="80" t="s">
+      <c r="J16" s="83" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
+      <c r="A17" s="74"/>
       <c r="B17" s="23">
         <v>8</v>
       </c>
@@ -2724,10 +3434,10 @@
       <c r="I17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="76"/>
+      <c r="J17" s="79"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="6">
         <v>9</v>
       </c>
@@ -2752,12 +3462,12 @@
       <c r="I18" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="J18" s="75" t="s">
+      <c r="J18" s="78" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="71"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="6"/>
       <c r="C19" s="17"/>
       <c r="D19" s="8" t="s">
@@ -2768,10 +3478,10 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="73"/>
+      <c r="J19" s="76"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="71"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="6"/>
       <c r="C20" s="17"/>
       <c r="D20" s="8" t="s">
@@ -2782,10 +3492,10 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="17"/>
-      <c r="J20" s="73"/>
+      <c r="J20" s="76"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="71"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="10">
         <v>10</v>
       </c>
@@ -2810,10 +3520,10 @@
       <c r="I21" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J21" s="73"/>
+      <c r="J21" s="76"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="71"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="6"/>
       <c r="C22" s="17"/>
       <c r="D22" s="7" t="s">
@@ -2826,10 +3536,10 @@
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="17"/>
-      <c r="J22" s="73"/>
+      <c r="J22" s="76"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="71"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="12"/>
       <c r="C23" s="19"/>
       <c r="D23" s="13"/>
@@ -2840,10 +3550,10 @@
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="76"/>
+      <c r="J23" s="79"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="71"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="6">
         <v>11</v>
       </c>
@@ -2871,7 +3581,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="71"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="10">
         <v>12</v>
       </c>
@@ -2892,12 +3602,12 @@
       <c r="I25" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="J25" s="75" t="s">
+      <c r="J25" s="78" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="12"/>
       <c r="C26" s="19"/>
       <c r="D26" s="13" t="s">
@@ -2908,10 +3618,10 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="19"/>
-      <c r="J26" s="76"/>
+      <c r="J26" s="79"/>
     </row>
     <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="72"/>
+      <c r="A27" s="75"/>
       <c r="B27" s="15">
         <v>13</v>
       </c>
@@ -2991,7 +3701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B63A016-4523-CA4C-A5E2-4AD2391F633B}">
   <dimension ref="A1:C18"/>
   <sheetViews>

</xml_diff>